<commit_message>
refs #661 Projektplan Grundgerüst
</commit_message>
<xml_diff>
--- a/doc/plan_ba.xlsx
+++ b/doc/plan_ba.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="17235" windowHeight="12075"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="17235" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="22">
   <si>
     <t>Abstract zur Kontrolle</t>
   </si>
@@ -59,6 +59,30 @@
   <si>
     <t>Woche 15 und 16 (nach Semersterschluss) als Reserve</t>
   </si>
+  <si>
+    <t>SP0</t>
+  </si>
+  <si>
+    <t>SP1</t>
+  </si>
+  <si>
+    <t>SP2</t>
+  </si>
+  <si>
+    <t>SP3</t>
+  </si>
+  <si>
+    <t>SP4</t>
+  </si>
+  <si>
+    <t>SP5</t>
+  </si>
+  <si>
+    <t>SP6</t>
+  </si>
+  <si>
+    <t>SP7</t>
+  </si>
 </sst>
 </file>
 
@@ -83,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,6 +117,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -109,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -152,6 +182,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M120"/>
+  <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,6 +519,9 @@
       <c r="D2" s="8">
         <v>40959</v>
       </c>
+      <c r="E2" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="L2" s="17" t="s">
         <v>9</v>
       </c>
@@ -508,6 +542,9 @@
       <c r="D3" s="8">
         <v>40960</v>
       </c>
+      <c r="E3" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="L3" s="17" t="s">
         <v>11</v>
       </c>
@@ -528,6 +565,9 @@
       <c r="D4" s="8">
         <v>40961</v>
       </c>
+      <c r="E4" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="K4" t="s">
         <v>13</v>
       </c>
@@ -545,6 +585,9 @@
       <c r="D5" s="8">
         <v>40962</v>
       </c>
+      <c r="E5" s="18" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
@@ -559,6 +602,9 @@
       <c r="D6" s="8">
         <v>40963</v>
       </c>
+      <c r="E6" s="18" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -573,6 +619,9 @@
       <c r="D7" s="8">
         <v>40964</v>
       </c>
+      <c r="E7" s="18" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
@@ -587,6 +636,9 @@
       <c r="D8" s="8">
         <v>40965</v>
       </c>
+      <c r="E8" s="18" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -601,6 +653,9 @@
       <c r="D9" s="2">
         <v>40966</v>
       </c>
+      <c r="E9" s="18" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -615,6 +670,9 @@
       <c r="D10" s="2">
         <v>40967</v>
       </c>
+      <c r="E10" s="18" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -629,6 +687,9 @@
       <c r="D11" s="2">
         <v>40968</v>
       </c>
+      <c r="E11" s="18" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -643,6 +704,9 @@
       <c r="D12" s="2">
         <v>40969</v>
       </c>
+      <c r="E12" s="18" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -657,6 +721,9 @@
       <c r="D13" s="2">
         <v>40970</v>
       </c>
+      <c r="E13" s="18" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -671,6 +738,9 @@
       <c r="D14" s="2">
         <v>40971</v>
       </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -685,6 +755,9 @@
       <c r="D15" s="2">
         <v>40972</v>
       </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
@@ -699,8 +772,11 @@
       <c r="D16" s="8">
         <v>40973</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>10</v>
       </c>
@@ -713,8 +789,11 @@
       <c r="D17" s="8">
         <v>40974</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>10</v>
       </c>
@@ -727,8 +806,11 @@
       <c r="D18" s="8">
         <v>40975</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>10</v>
       </c>
@@ -741,8 +823,11 @@
       <c r="D19" s="8">
         <v>40976</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>10</v>
       </c>
@@ -755,8 +840,11 @@
       <c r="D20" s="8">
         <v>40977</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>10</v>
       </c>
@@ -769,8 +857,11 @@
       <c r="D21" s="8">
         <v>40978</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>10</v>
       </c>
@@ -783,8 +874,11 @@
       <c r="D22" s="8">
         <v>40979</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>11</v>
       </c>
@@ -797,8 +891,11 @@
       <c r="D23" s="2">
         <v>40980</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>11</v>
       </c>
@@ -811,8 +908,11 @@
       <c r="D24" s="2">
         <v>40981</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>11</v>
       </c>
@@ -825,8 +925,11 @@
       <c r="D25" s="2">
         <v>40982</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>11</v>
       </c>
@@ -839,8 +942,11 @@
       <c r="D26" s="2">
         <v>40983</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>11</v>
       </c>
@@ -853,8 +959,11 @@
       <c r="D27" s="2">
         <v>40984</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>11</v>
       </c>
@@ -867,8 +976,11 @@
       <c r="D28" s="2">
         <v>40985</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>11</v>
       </c>
@@ -881,8 +993,11 @@
       <c r="D29" s="2">
         <v>40986</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>12</v>
       </c>
@@ -895,8 +1010,11 @@
       <c r="D30" s="8">
         <v>40987</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>12</v>
       </c>
@@ -909,8 +1027,11 @@
       <c r="D31" s="8">
         <v>40988</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>12</v>
       </c>
@@ -922,6 +1043,9 @@
       </c>
       <c r="D32" s="8">
         <v>40989</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -937,6 +1061,9 @@
       <c r="D33" s="8">
         <v>40990</v>
       </c>
+      <c r="E33" s="18" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
@@ -951,6 +1078,9 @@
       <c r="D34" s="8">
         <v>40991</v>
       </c>
+      <c r="E34" s="18" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
@@ -965,6 +1095,9 @@
       <c r="D35" s="8">
         <v>40992</v>
       </c>
+      <c r="E35" s="18" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
@@ -979,6 +1112,9 @@
       <c r="D36" s="8">
         <v>40993</v>
       </c>
+      <c r="E36" s="18" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
@@ -993,6 +1129,9 @@
       <c r="D37" s="2">
         <v>40994</v>
       </c>
+      <c r="E37" s="18" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
@@ -1007,6 +1146,9 @@
       <c r="D38" s="2">
         <v>40995</v>
       </c>
+      <c r="E38" s="18" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
@@ -1021,6 +1163,9 @@
       <c r="D39" s="2">
         <v>40996</v>
       </c>
+      <c r="E39" s="18" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
@@ -1035,6 +1180,9 @@
       <c r="D40" s="2">
         <v>40997</v>
       </c>
+      <c r="E40" s="18" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
@@ -1049,6 +1197,9 @@
       <c r="D41" s="2">
         <v>40998</v>
       </c>
+      <c r="E41" s="18" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
@@ -1063,6 +1214,9 @@
       <c r="D42" s="2">
         <v>40999</v>
       </c>
+      <c r="E42" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
@@ -1077,6 +1231,9 @@
       <c r="D43" s="2">
         <v>41000</v>
       </c>
+      <c r="E43" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
@@ -1091,6 +1248,9 @@
       <c r="D44" s="8">
         <v>41001</v>
       </c>
+      <c r="E44" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
@@ -1105,6 +1265,9 @@
       <c r="D45" s="8">
         <v>41002</v>
       </c>
+      <c r="E45" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
@@ -1119,6 +1282,9 @@
       <c r="D46" s="8">
         <v>41003</v>
       </c>
+      <c r="E46" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
@@ -1133,6 +1299,9 @@
       <c r="D47" s="8">
         <v>41004</v>
       </c>
+      <c r="E47" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
@@ -1148,9 +1317,11 @@
         <v>41005</v>
       </c>
       <c r="E48" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F48" s="13"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
@@ -1166,9 +1337,11 @@
         <v>41006</v>
       </c>
       <c r="E49" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F49" s="13"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
@@ -1184,9 +1357,11 @@
         <v>41007</v>
       </c>
       <c r="E50" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F50" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F50" s="13"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="14">
@@ -1202,9 +1377,11 @@
         <v>41008</v>
       </c>
       <c r="E51" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F51" s="13"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="14">
@@ -1220,9 +1397,11 @@
         <v>41009</v>
       </c>
       <c r="E52" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F52" s="13"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
@@ -1237,6 +1416,9 @@
       <c r="D53" s="2">
         <v>41010</v>
       </c>
+      <c r="E53" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
@@ -1251,6 +1433,9 @@
       <c r="D54" s="2">
         <v>41011</v>
       </c>
+      <c r="E54" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
@@ -1265,6 +1450,9 @@
       <c r="D55" s="2">
         <v>41012</v>
       </c>
+      <c r="E55" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
@@ -1279,6 +1467,9 @@
       <c r="D56" s="2">
         <v>41013</v>
       </c>
+      <c r="E56" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
@@ -1292,6 +1483,9 @@
       </c>
       <c r="D57" s="2">
         <v>41014</v>
+      </c>
+      <c r="E57" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1307,6 +1501,9 @@
       <c r="D58" s="8">
         <v>41015</v>
       </c>
+      <c r="E58" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
@@ -1321,6 +1518,9 @@
       <c r="D59" s="8">
         <v>41016</v>
       </c>
+      <c r="E59" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
@@ -1335,6 +1535,9 @@
       <c r="D60" s="8">
         <v>41017</v>
       </c>
+      <c r="E60" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
@@ -1349,6 +1552,9 @@
       <c r="D61" s="8">
         <v>41018</v>
       </c>
+      <c r="E61" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
@@ -1363,6 +1569,9 @@
       <c r="D62" s="8">
         <v>41019</v>
       </c>
+      <c r="E62" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
@@ -1377,6 +1586,9 @@
       <c r="D63" s="8">
         <v>41020</v>
       </c>
+      <c r="E63" s="18" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
@@ -1391,8 +1603,11 @@
       <c r="D64" s="8">
         <v>41021</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>17</v>
       </c>
@@ -1405,8 +1620,11 @@
       <c r="D65" s="2">
         <v>41022</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>17</v>
       </c>
@@ -1419,8 +1637,11 @@
       <c r="D66" s="2">
         <v>41023</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>17</v>
       </c>
@@ -1433,8 +1654,11 @@
       <c r="D67" s="2">
         <v>41024</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>17</v>
       </c>
@@ -1447,8 +1671,11 @@
       <c r="D68" s="2">
         <v>41025</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>17</v>
       </c>
@@ -1461,8 +1688,11 @@
       <c r="D69" s="2">
         <v>41026</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>17</v>
       </c>
@@ -1475,8 +1705,11 @@
       <c r="D70" s="2">
         <v>41027</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>17</v>
       </c>
@@ -1489,8 +1722,11 @@
       <c r="D71" s="2">
         <v>41028</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <v>18</v>
       </c>
@@ -1503,8 +1739,11 @@
       <c r="D72" s="8">
         <v>41029</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>18</v>
       </c>
@@ -1517,8 +1756,11 @@
       <c r="D73" s="8">
         <v>41030</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>18</v>
       </c>
@@ -1531,8 +1773,11 @@
       <c r="D74" s="8">
         <v>41031</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>18</v>
       </c>
@@ -1545,8 +1790,11 @@
       <c r="D75" s="8">
         <v>41032</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>18</v>
       </c>
@@ -1559,8 +1807,11 @@
       <c r="D76" s="8">
         <v>41033</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <v>18</v>
       </c>
@@ -1573,8 +1824,11 @@
       <c r="D77" s="8">
         <v>41034</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <v>18</v>
       </c>
@@ -1587,8 +1841,11 @@
       <c r="D78" s="8">
         <v>41035</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>19</v>
       </c>
@@ -1601,8 +1858,11 @@
       <c r="D79" s="2">
         <v>41036</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>19</v>
       </c>
@@ -1615,8 +1875,11 @@
       <c r="D80" s="2">
         <v>41037</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>19</v>
       </c>
@@ -1629,8 +1892,11 @@
       <c r="D81" s="2">
         <v>41038</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>19</v>
       </c>
@@ -1643,8 +1909,11 @@
       <c r="D82" s="2">
         <v>41039</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>19</v>
       </c>
@@ -1657,8 +1926,11 @@
       <c r="D83" s="2">
         <v>41040</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>19</v>
       </c>
@@ -1671,8 +1943,11 @@
       <c r="D84" s="2">
         <v>41041</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E84" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>19</v>
       </c>
@@ -1685,8 +1960,11 @@
       <c r="D85" s="2">
         <v>41042</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E85" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
         <v>20</v>
       </c>
@@ -1699,8 +1977,11 @@
       <c r="D86" s="8">
         <v>41043</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
         <v>20</v>
       </c>
@@ -1713,8 +1994,11 @@
       <c r="D87" s="8">
         <v>41044</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="6">
         <v>20</v>
       </c>
@@ -1727,8 +2011,11 @@
       <c r="D88" s="8">
         <v>41045</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="10">
         <v>20</v>
       </c>
@@ -1741,11 +2028,14 @@
       <c r="D89" s="12">
         <v>41046</v>
       </c>
-      <c r="E89" s="13" t="s">
+      <c r="E89" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
         <v>20</v>
       </c>
@@ -1758,8 +2048,11 @@
       <c r="D90" s="8">
         <v>41047</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E90" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="6">
         <v>20</v>
       </c>
@@ -1772,8 +2065,11 @@
       <c r="D91" s="8">
         <v>41048</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E91" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
         <v>20</v>
       </c>
@@ -1786,8 +2082,11 @@
       <c r="D92" s="8">
         <v>41049</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>21</v>
       </c>
@@ -1800,8 +2099,11 @@
       <c r="D93" s="2">
         <v>41050</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>21</v>
       </c>
@@ -1814,8 +2116,11 @@
       <c r="D94" s="2">
         <v>41051</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>21</v>
       </c>
@@ -1828,8 +2133,11 @@
       <c r="D95" s="2">
         <v>41052</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>21</v>
       </c>
@@ -1842,8 +2150,11 @@
       <c r="D96" s="2">
         <v>41053</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E96" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>21</v>
       </c>
@@ -1856,8 +2167,11 @@
       <c r="D97" s="2">
         <v>41054</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>21</v>
       </c>
@@ -1870,8 +2184,11 @@
       <c r="D98" s="2">
         <v>41055</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E98" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>21</v>
       </c>
@@ -1884,8 +2201,11 @@
       <c r="D99" s="2">
         <v>41056</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E99" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="10">
         <v>22</v>
       </c>
@@ -1898,11 +2218,14 @@
       <c r="D100" s="12">
         <v>41057</v>
       </c>
-      <c r="E100" s="13" t="s">
+      <c r="E100" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F100" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="6">
         <v>22</v>
       </c>
@@ -1915,8 +2238,11 @@
       <c r="D101" s="8">
         <v>41058</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E101" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="6">
         <v>22</v>
       </c>
@@ -1929,8 +2255,11 @@
       <c r="D102" s="8">
         <v>41059</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E102" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
         <v>22</v>
       </c>
@@ -1943,8 +2272,11 @@
       <c r="D103" s="8">
         <v>41060</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E103" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
         <v>22</v>
       </c>
@@ -1957,11 +2289,14 @@
       <c r="D104" s="8">
         <v>41061</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E104" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F104" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="6">
         <v>22</v>
       </c>
@@ -1974,8 +2309,11 @@
       <c r="D105" s="8">
         <v>41062</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E105" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="6">
         <v>22</v>
       </c>
@@ -1988,8 +2326,11 @@
       <c r="D106" s="8">
         <v>41063</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E106" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>23</v>
       </c>
@@ -2002,8 +2343,11 @@
       <c r="D107" s="2">
         <v>41064</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E107" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>23</v>
       </c>
@@ -2016,8 +2360,11 @@
       <c r="D108" s="2">
         <v>41065</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E108" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>23</v>
       </c>
@@ -2030,8 +2377,11 @@
       <c r="D109" s="2">
         <v>41066</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E109" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>23</v>
       </c>
@@ -2044,8 +2394,11 @@
       <c r="D110" s="2">
         <v>41067</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E110" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>23</v>
       </c>
@@ -2059,10 +2412,13 @@
         <v>41068</v>
       </c>
       <c r="E111" t="s">
+        <v>21</v>
+      </c>
+      <c r="F111" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>23</v>
       </c>
@@ -2075,8 +2431,11 @@
       <c r="D112" s="2">
         <v>41069</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E112" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>23</v>
       </c>
@@ -2089,8 +2448,11 @@
       <c r="D113" s="2">
         <v>41070</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E113" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="6">
         <v>24</v>
       </c>
@@ -2103,8 +2465,11 @@
       <c r="D114" s="8">
         <v>41071</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E114" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="6">
         <v>24</v>
       </c>
@@ -2117,8 +2482,11 @@
       <c r="D115" s="8">
         <v>41072</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E115" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="6">
         <v>24</v>
       </c>
@@ -2131,8 +2499,11 @@
       <c r="D116" s="8">
         <v>41073</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E116" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="6">
         <v>24</v>
       </c>
@@ -2145,8 +2516,11 @@
       <c r="D117" s="8">
         <v>41074</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E117" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="6">
         <v>24</v>
       </c>
@@ -2160,35 +2534,10 @@
         <v>41075</v>
       </c>
       <c r="E118" t="s">
+        <v>21</v>
+      </c>
+      <c r="F118" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="6">
-        <v>24</v>
-      </c>
-      <c r="B119" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C119" s="7">
-        <v>41076</v>
-      </c>
-      <c r="D119" s="8">
-        <v>41076</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="6">
-        <v>24</v>
-      </c>
-      <c r="B120" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C120" s="7">
-        <v>41077</v>
-      </c>
-      <c r="D120" s="8">
-        <v>41077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>